<commit_message>
Updated changelog with ruleset changes from Mike (PWRE) sent on March 19, 2018.
</commit_message>
<xml_diff>
--- a/MTOM_System_Changelog.xlsx
+++ b/MTOM_System_Changelog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="179">
   <si>
     <t>Index</t>
   </si>
@@ -4706,6 +4706,235 @@
   </si>
   <si>
     <t>1.) Edited contact information in the "Information" button  2.) Deleted exit button so that done button more clearly means data will be implemented  3.) Replaced direct database connections with API queries to bring in 24MS data</t>
+  </si>
+  <si>
+    <t>MTOM_Rules_FEB18_Update20180309.rls.gz</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.) Moved Development Notes for all rules &amp; functions from the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field of the Rule Editor window to the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Notes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field; 2.) Added </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Drivers of Operations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> descriptions to Policy Groups in ruleset; 3.) Removed additional outdated and/or unused rules and functions: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TaylorParkMaxReleaseConstraint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CalcGunnisonShoulderFlowTarget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CalcGunnisonPeakFlowLevel_OLD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CalcGunnisonPeakFlowTarget_OLD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CalcCanyonPeakFlowTarget_OLD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DeliveryCAICS_SacWY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GetIndexYearDailyList_pre201707</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GetCurrentYearDailyList_pre201707</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5049,7 +5278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5178,11 +5407,60 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -5256,43 +5534,6 @@
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -5423,7 +5664,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5491,7 +5732,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5559,7 +5800,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5627,7 +5868,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5695,7 +5936,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5760,8 +6001,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tableRules" displayName="tableRules" ref="A1:E35" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:E35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tableRules" displayName="tableRules" ref="A1:E36" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E36"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Index" dataDxfId="4"/>
+    <tableColumn id="2" name="Date" dataDxfId="3"/>
+    <tableColumn id="3" name="Author" dataDxfId="2"/>
+    <tableColumn id="4" name="Filename" dataDxfId="1"/>
+    <tableColumn id="5" name="Description" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tableForecast" displayName="tableForecast" ref="A1:E4" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Index" dataDxfId="22"/>
     <tableColumn id="2" name="Date" dataDxfId="21"/>
@@ -5769,32 +6024,18 @@
     <tableColumn id="4" name="Filename" dataDxfId="19"/>
     <tableColumn id="5" name="Description" dataDxfId="18"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tableForecast" displayName="tableForecast" ref="A1:E4" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:E4"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tableOutput" displayName="tableOutput" ref="A1:E11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:E11"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Index" dataDxfId="15"/>
     <tableColumn id="2" name="Date" dataDxfId="14"/>
     <tableColumn id="3" name="Author" dataDxfId="13"/>
     <tableColumn id="4" name="Filename" dataDxfId="12"/>
-    <tableColumn id="5" name="Description" dataDxfId="11"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tableOutput" displayName="tableOutput" ref="A1:E11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:E11"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Index" dataDxfId="8"/>
-    <tableColumn id="2" name="Date" dataDxfId="7"/>
-    <tableColumn id="3" name="Author" dataDxfId="6"/>
-    <tableColumn id="4" name="Filename" dataDxfId="5"/>
     <tableColumn id="5" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5802,13 +6043,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tableCompare" displayName="tableCompare" ref="A1:E2" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tableCompare" displayName="tableCompare" ref="A1:E2" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Index" dataDxfId="3"/>
-    <tableColumn id="2" name="Date" dataDxfId="2"/>
-    <tableColumn id="3" name="Author" dataDxfId="1"/>
-    <tableColumn id="4" name="Filename" dataDxfId="0"/>
+    <tableColumn id="1" name="Index" dataDxfId="10"/>
+    <tableColumn id="2" name="Date" dataDxfId="9"/>
+    <tableColumn id="3" name="Author" dataDxfId="8"/>
+    <tableColumn id="4" name="Filename" dataDxfId="7"/>
     <tableColumn id="5" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6737,11 +6978,11 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E38:E39"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7351,6 +7592,21 @@
       </c>
       <c r="E35" s="45" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="48"/>
+      <c r="B36" s="49">
+        <v>43168</v>
+      </c>
+      <c r="C36" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="51" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="50" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -7369,7 +7625,7 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>